<commit_message>
all files need to be updated
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ODBM\our-daily-bread-ministry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ODBM\OurDailyBreadMinistry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1B3AEA-8CEB-424F-B283-A76C59083B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754D97A0-F9C0-48A3-A0A6-08776AAC25C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{06B77847-E926-4A05-B4DF-44B4F755AE6A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Email</t>
   </si>
@@ -46,13 +46,25 @@
   </si>
   <si>
     <t>Company</t>
+  </si>
+  <si>
+    <t>captain@gmail.com</t>
+  </si>
+  <si>
+    <t>Archer</t>
+  </si>
+  <si>
+    <t>jofra</t>
+  </si>
+  <si>
+    <t>3 lions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +76,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,14 +106,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -110,9 +133,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -150,7 +173,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -256,7 +279,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -398,7 +421,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -406,18 +429,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B83B128E-E352-4E35-970D-3C80CEA1EED0}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.77734375" customWidth="1"/>
     <col min="2" max="2" width="22.44140625" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
@@ -434,8 +457,25 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{13E24231-5D14-4974-A4CB-A1325614D476}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>